<commit_message>
Résultat session du 02/11/2025 de 9h à 11h.
</commit_message>
<xml_diff>
--- a/docs/features/All_Features.xlsx
+++ b/docs/features/All_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malikchettih/Projects/Emiasd-Projects/Emiasd-FlightProject/docs/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAAA5E5-C7AC-2A40-BDB4-6BAB7127252C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D89697-8920-B945-B18A-E3428F720E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20900" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{48A1BF46-FD0F-4445-B897-6B2410F84F78}"/>
+    <workbookView xWindow="17520" yWindow="-18060" windowWidth="38400" windowHeight="19900" activeTab="6" xr2:uid="{48A1BF46-FD0F-4445-B897-6B2410F84F78}"/>
   </bookViews>
   <sheets>
     <sheet name="Fligh" sheetId="3" r:id="rId1"/>
@@ -2456,15 +2456,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>97693</xdr:colOff>
+      <xdr:colOff>457526</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>205764</xdr:rowOff>
+      <xdr:rowOff>184597</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>736601</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>270934</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>69361</xdr:rowOff>
+      <xdr:rowOff>48194</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2487,8 +2487,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11381155" y="420687"/>
-          <a:ext cx="3960446" cy="2227751"/>
+          <a:off x="11728776" y="396264"/>
+          <a:ext cx="3940908" cy="2191930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2500,13 +2500,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>175846</xdr:colOff>
+      <xdr:colOff>451013</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>214922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
+      <xdr:colOff>363090</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>155905</xdr:rowOff>
     </xdr:to>
@@ -2531,8 +2531,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11459308" y="2793999"/>
-          <a:ext cx="4064000" cy="1670137"/>
+          <a:off x="11722263" y="2754922"/>
+          <a:ext cx="4039577" cy="1655483"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2543,16 +2543,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>572315</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>699315</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>53836</xdr:rowOff>
+      <xdr:rowOff>22086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>587945</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>29795</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>714945</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2575,7 +2575,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15145565" y="477169"/>
+          <a:off x="16098065" y="445419"/>
           <a:ext cx="2492130" cy="1669293"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2588,15 +2588,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>214922</xdr:colOff>
+      <xdr:colOff>437172</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>161517</xdr:rowOff>
+      <xdr:rowOff>225017</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>361460</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>187569</xdr:rowOff>
+      <xdr:colOff>583710</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>39402</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2619,8 +2619,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11498384" y="4469748"/>
-          <a:ext cx="4298461" cy="1110436"/>
+          <a:off x="11708422" y="4479517"/>
+          <a:ext cx="4274038" cy="1105552"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2632,15 +2632,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>215487</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>48847</xdr:rowOff>
+      <xdr:colOff>247237</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>27681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>417424</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>166077</xdr:rowOff>
+      <xdr:colOff>449174</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>123743</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2663,8 +2663,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11498949" y="5656385"/>
-          <a:ext cx="3523475" cy="3556000"/>
+          <a:off x="11518487" y="5785014"/>
+          <a:ext cx="3503937" cy="3503896"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2675,16 +2675,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>732693</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>39077</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>595109</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>81411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>664368</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>526784</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>52918</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2707,8 +2707,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14507308" y="5646615"/>
-          <a:ext cx="3253214" cy="3624386"/>
+          <a:off x="15168359" y="5838744"/>
+          <a:ext cx="3233675" cy="3580424"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3275,7 +3275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8048ADBB-B888-444A-B15B-F1F4566FE49D}">
   <dimension ref="B2:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -6102,8 +6102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20F12E2-3AEB-8A4D-B17B-B4DD117D6CE4}">
   <dimension ref="B1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C43"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>